<commit_message>
Reproduce #1165 with 'a reliable series of steps'
</commit_message>
<xml_diff>
--- a/tests/core/exports/books.xlsx
+++ b/tests/core/exports/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added</t>
   </si>
   <si>
     <t xml:space="preserve">Some book</t>
@@ -44,8 +47,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -119,12 +123,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -145,13 +157,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.29"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -163,8 +178,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -172,20 +190,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <f aca="false">ABS(-4)</f>
         <v>4</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>43988.5</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>